<commit_message>
Fixed Swap Column Problems in the Main Chart. Updated to 1.6r.
</commit_message>
<xml_diff>
--- a/MonthlyReportCollector/Assets/MSP新版月报模板.xlsx
+++ b/MonthlyReportCollector/Assets/MSP新版月报模板.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$1</definedName>
   </definedNames>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -319,7 +319,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>活动那个内容网盘链接</t>
+    <t>活动内容网盘链接</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -802,37 +802,37 @@
   <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="X1" sqref="X1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="25.5" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.25" style="6" customWidth="1"/>
-    <col min="2" max="3" width="12.83203125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="28.83203125" style="6" customWidth="1"/>
+    <col min="2" max="3" width="12.875" style="6" customWidth="1"/>
+    <col min="4" max="4" width="28.875" style="6" customWidth="1"/>
     <col min="5" max="5" width="16.25" style="6" customWidth="1"/>
     <col min="6" max="6" width="20.75" style="6" customWidth="1"/>
-    <col min="7" max="7" width="13.83203125" style="6" customWidth="1"/>
-    <col min="8" max="8" width="16.33203125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="13.875" style="6" customWidth="1"/>
+    <col min="8" max="8" width="16.375" style="6" customWidth="1"/>
     <col min="9" max="10" width="14.75" style="6" customWidth="1"/>
     <col min="11" max="11" width="18.75" style="5" customWidth="1"/>
-    <col min="12" max="12" width="14.33203125" style="6" customWidth="1"/>
-    <col min="13" max="13" width="49.83203125" style="6" customWidth="1"/>
+    <col min="12" max="12" width="14.375" style="6" customWidth="1"/>
+    <col min="13" max="13" width="49.875" style="6" customWidth="1"/>
     <col min="14" max="14" width="13.25" style="1" customWidth="1"/>
     <col min="15" max="15" width="18.25" style="6" customWidth="1"/>
     <col min="16" max="16" width="11.5" style="1" customWidth="1"/>
-    <col min="17" max="17" width="19.83203125" style="6" customWidth="1"/>
-    <col min="18" max="18" width="11.08203125" style="1" customWidth="1"/>
-    <col min="19" max="19" width="41.83203125" style="6" customWidth="1"/>
+    <col min="17" max="17" width="19.875" style="6" customWidth="1"/>
+    <col min="18" max="18" width="11.125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="41.875" style="6" customWidth="1"/>
     <col min="20" max="20" width="17" style="1" customWidth="1"/>
     <col min="21" max="21" width="19.75" style="6" customWidth="1"/>
     <col min="22" max="22" width="17.75" style="1" customWidth="1"/>
-    <col min="23" max="23" width="18.83203125" style="6" customWidth="1"/>
+    <col min="23" max="23" width="18.875" style="6" customWidth="1"/>
     <col min="24" max="24" width="21" style="1" customWidth="1"/>
     <col min="25" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -906,7 +906,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">

</xml_diff>